<commit_message>
completed  Expense Tracker Project
</commit_message>
<xml_diff>
--- a/server/expense.details.xlsx
+++ b/server/expense.details.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="expense" sheetId="1" r:id="rId1"/>
+    <sheet name="Expense" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -64,8 +64,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,13 +398,168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Icon</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Category</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Amount</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Date</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>💡</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Utilities</v>
+      </c>
+      <c r="C2">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="1">
+        <v>45862.22928240741</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>🛒</v>
+      </c>
+      <c r="B3" t="str">
+        <v>me</v>
+      </c>
+      <c r="C3">
+        <v>1200</v>
+      </c>
+      <c r="D3" s="1">
+        <v>45862.22928240741</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>🛒</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Groceries</v>
+      </c>
+      <c r="C4">
+        <v>2500</v>
+      </c>
+      <c r="D4" s="1">
+        <v>45861.22928240741</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>💡</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Electricity Bill</v>
+      </c>
+      <c r="C5">
+        <v>13000</v>
+      </c>
+      <c r="D5" s="1">
+        <v>45845.22928240741</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>🎬</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Entertainment</v>
+      </c>
+      <c r="C6">
+        <v>750</v>
+      </c>
+      <c r="D6" s="1">
+        <v>45843.22928240741</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>🏠</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Rent</v>
+      </c>
+      <c r="C7">
+        <v>9500</v>
+      </c>
+      <c r="D7" s="1">
+        <v>45841.22928240741</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>🚗</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Transport</v>
+      </c>
+      <c r="C8">
+        <v>1200</v>
+      </c>
+      <c r="D8" s="1">
+        <v>45840.22928240741</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>🚕</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Transport</v>
+      </c>
+      <c r="C9">
+        <v>120</v>
+      </c>
+      <c r="D9" s="1">
+        <v>45840.22928240741</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>🍔</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C10">
+        <v>450</v>
+      </c>
+      <c r="D10" s="1">
+        <v>45839.22928240741</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>🍕</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C11">
+        <v>350</v>
+      </c>
+      <c r="D11" s="1">
+        <v>45839.22928240741</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>